<commit_message>
updated category scoring config to include all classified categories
</commit_message>
<xml_diff>
--- a/backend/data/category_scoring_config.xlsx
+++ b/backend/data/category_scoring_config.xlsx
@@ -8,12 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anye forti\Desktop\Projects\clarity-cash\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1183E4-B691-49B0-B25C-16629AAD20F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95126B76-45DC-432B-AE17-D8C6362C03BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14370" yWindow="135" windowWidth="14190" windowHeight="16200" xr2:uid="{1750716D-C456-49B0-8BF2-ED871E7EA8A9}"/>
+    <workbookView xWindow="960" yWindow="180" windowWidth="14190" windowHeight="16200" firstSheet="3" activeTab="4" xr2:uid="{1750716D-C456-49B0-8BF2-ED871E7EA8A9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="CAT_LABELS" sheetId="1" r:id="rId1"/>
+    <sheet name="PROFILE" sheetId="3" r:id="rId2"/>
+    <sheet name="SPEND_PROF_CATEGORY" sheetId="2" r:id="rId3"/>
+    <sheet name="CONTEXT" sheetId="4" r:id="rId4"/>
+    <sheet name="CONTEXT_CATEGORY" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>CAT_ID</t>
   </si>
@@ -45,6 +49,51 @@
   </si>
   <si>
     <t>AFFECTS_SCORES</t>
+  </si>
+  <si>
+    <t>PROF_ID</t>
+  </si>
+  <si>
+    <t>SAVINGS_POSITIVE</t>
+  </si>
+  <si>
+    <t>NEGATIVE_EVENTS</t>
+  </si>
+  <si>
+    <t>FLEX_ESSENTIAL</t>
+  </si>
+  <si>
+    <t>DISCRETIONARY_WANT</t>
+  </si>
+  <si>
+    <t>CONTEXT_ID</t>
+  </si>
+  <si>
+    <t>SPEND_PROF_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>CONTEXT_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>EFFECTIVE_INCOME</t>
+  </si>
+  <si>
+    <t>SAVINGS_CONTEXT</t>
+  </si>
+  <si>
+    <t>EMERGENCY_BORROWING</t>
+  </si>
+  <si>
+    <t>FEES_CONTEXT</t>
+  </si>
+  <si>
+    <t>STRUCTURAL_UNAVOIDABLE</t>
+  </si>
+  <si>
+    <t>FLEX_CORE_ESSENTIAL</t>
+  </si>
+  <si>
+    <t>FLEX_OTHER_ESSENTIAL</t>
   </si>
 </sst>
 </file>
@@ -422,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3856665D-78B6-4A19-8191-194CE6C00A53}">
   <dimension ref="A1:C105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E105" sqref="E105"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1584,6 +1633,1043 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C105">
+    <sortCondition ref="A1:A105"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01A0D34D-34B6-4B74-B93F-533A65FB1CFD}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF8E169C-0644-47E0-B002-A7E43E9D531A}">
+  <dimension ref="A1:B58"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>26</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>27</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>28</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>29</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>30</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>31</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>32</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>33</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>34</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>35</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>36</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>37</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>38</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>39</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>40</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>41</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>42</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>43</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>44</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>45</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>46</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>47</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>48</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>49</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>50</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>51</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>52</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>53</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>54</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>55</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>56</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>57</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>58</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>59</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>60</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>61</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>62</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>70</v>
+      </c>
+      <c r="B42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>71</v>
+      </c>
+      <c r="B43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>72</v>
+      </c>
+      <c r="B44">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>73</v>
+      </c>
+      <c r="B45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>74</v>
+      </c>
+      <c r="B46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>80</v>
+      </c>
+      <c r="B47">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>81</v>
+      </c>
+      <c r="B48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>82</v>
+      </c>
+      <c r="B49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>83</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>87</v>
+      </c>
+      <c r="B51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>88</v>
+      </c>
+      <c r="B52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>89</v>
+      </c>
+      <c r="B53">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>91</v>
+      </c>
+      <c r="B54">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>94</v>
+      </c>
+      <c r="B55">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>95</v>
+      </c>
+      <c r="B56">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>96</v>
+      </c>
+      <c r="B57">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>97</v>
+      </c>
+      <c r="B58">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A0B0A54-EBD8-4483-8003-BDECA55AA08A}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{550B3CE6-B11A-4F82-9FAE-C2294524CC09}">
+  <dimension ref="A1:B51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>19</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>21</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>22</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>23</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>24</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>25</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>26</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>27</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>28</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>29</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>30</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>40</v>
+      </c>
+      <c r="B25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>63</v>
+      </c>
+      <c r="B26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>64</v>
+      </c>
+      <c r="B27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>65</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>66</v>
+      </c>
+      <c r="B29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>67</v>
+      </c>
+      <c r="B30">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>68</v>
+      </c>
+      <c r="B31">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>69</v>
+      </c>
+      <c r="B32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>75</v>
+      </c>
+      <c r="B33">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>76</v>
+      </c>
+      <c r="B34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>77</v>
+      </c>
+      <c r="B35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>78</v>
+      </c>
+      <c r="B36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>79</v>
+      </c>
+      <c r="B37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>84</v>
+      </c>
+      <c r="B38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>85</v>
+      </c>
+      <c r="B39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>86</v>
+      </c>
+      <c r="B40">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>88</v>
+      </c>
+      <c r="B41">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>90</v>
+      </c>
+      <c r="B42">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>92</v>
+      </c>
+      <c r="B43">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>93</v>
+      </c>
+      <c r="B44">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>98</v>
+      </c>
+      <c r="B45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>99</v>
+      </c>
+      <c r="B46">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>100</v>
+      </c>
+      <c r="B47">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>101</v>
+      </c>
+      <c r="B48">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>102</v>
+      </c>
+      <c r="B49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>103</v>
+      </c>
+      <c r="B50">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>104</v>
+      </c>
+      <c r="B51">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
created scoring config + fixed data
</commit_message>
<xml_diff>
--- a/backend/data/category_scoring_config.xlsx
+++ b/backend/data/category_scoring_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anye forti\Desktop\Projects\clarity-cash\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95126B76-45DC-432B-AE17-D8C6362C03BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02833292-54E1-40DA-8673-862E4C445FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="180" windowWidth="14190" windowHeight="16200" firstSheet="3" activeTab="4" xr2:uid="{1750716D-C456-49B0-8BF2-ED871E7EA8A9}"/>
+    <workbookView xWindow="11625" yWindow="315" windowWidth="14190" windowHeight="16200" firstSheet="1" activeTab="3" xr2:uid="{1750716D-C456-49B0-8BF2-ED871E7EA8A9}"/>
   </bookViews>
   <sheets>
     <sheet name="CAT_LABELS" sheetId="1" r:id="rId1"/>
@@ -69,12 +69,6 @@
     <t>CONTEXT_ID</t>
   </si>
   <si>
-    <t>SPEND_PROF_DESCRIPTION</t>
-  </si>
-  <si>
-    <t>CONTEXT_DESCRIPTION</t>
-  </si>
-  <si>
     <t>EFFECTIVE_INCOME</t>
   </si>
   <si>
@@ -95,14 +89,17 @@
   <si>
     <t>FLEX_OTHER_ESSENTIAL</t>
   </si>
+  <si>
+    <t>SPEND_PROFILE</t>
+  </si>
+  <si>
+    <t>CONTEXT_BUCKET</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="000"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -132,9 +129,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,7 +468,7 @@
   <dimension ref="A1:C105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,338 +485,338 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
+      <c r="A2">
+        <v>510</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
+      <c r="A3">
+        <v>511</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
+      <c r="A4">
+        <v>512</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
+      <c r="A5">
+        <v>513</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
+      <c r="A6">
+        <v>516</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
+      <c r="A7">
+        <v>517</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7</v>
+      <c r="A8">
+        <v>518</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>8</v>
+      <c r="A9">
+        <v>531</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>9</v>
+      <c r="A10">
+        <v>532</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>10</v>
+      <c r="A11">
+        <v>533</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>11</v>
+      <c r="A12">
+        <v>534</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>12</v>
+      <c r="A13">
+        <v>535</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>13</v>
+      <c r="A14">
+        <v>536</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>14</v>
+      <c r="A15">
+        <v>537</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>15</v>
+      <c r="A16">
+        <v>538</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>16</v>
+      <c r="A17">
+        <v>539</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>17</v>
+      <c r="A18">
+        <v>541</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>18</v>
+      <c r="A19">
+        <v>542</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>19</v>
+      <c r="A20">
+        <v>543</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>20</v>
+      <c r="A21">
+        <v>544</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>21</v>
+      <c r="A22">
+        <v>545</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>22</v>
+      <c r="A23">
+        <v>546</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>23</v>
+      <c r="A24">
+        <v>547</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>24</v>
+      <c r="A25">
+        <v>548</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>25</v>
+      <c r="A26">
+        <v>549</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>26</v>
+      <c r="A27">
+        <v>550</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>27</v>
+      <c r="A28">
+        <v>551</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>28</v>
+      <c r="A29">
+        <v>552</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>29</v>
+      <c r="A30">
+        <v>553</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>30</v>
+      <c r="A31">
+        <v>554</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>31</v>
+      <c r="A32">
+        <v>555</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -830,8 +826,8 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>32</v>
+      <c r="A33">
+        <v>556</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -841,8 +837,8 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>33</v>
+      <c r="A34">
+        <v>557</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -852,8 +848,8 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>34</v>
+      <c r="A35">
+        <v>558</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -863,8 +859,8 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>35</v>
+      <c r="A36">
+        <v>559</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -874,8 +870,8 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <v>36</v>
+      <c r="A37">
+        <v>560</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -885,8 +881,8 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
-        <v>37</v>
+      <c r="A38">
+        <v>561</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -896,8 +892,8 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <v>38</v>
+      <c r="A39">
+        <v>562</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -907,8 +903,8 @@
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
-        <v>39</v>
+      <c r="A40">
+        <v>570</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -918,19 +914,19 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <v>40</v>
+      <c r="A41">
+        <v>571</v>
       </c>
       <c r="B41">
         <v>1</v>
       </c>
       <c r="C41">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
-        <v>41</v>
+      <c r="A42">
+        <v>572</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -940,8 +936,8 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
-        <v>42</v>
+      <c r="A43">
+        <v>573</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -951,8 +947,8 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
-        <v>43</v>
+      <c r="A44">
+        <v>574</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -962,8 +958,8 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
-        <v>44</v>
+      <c r="A45">
+        <v>580</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -973,8 +969,8 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
-        <v>45</v>
+      <c r="A46">
+        <v>581</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -984,8 +980,8 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
-        <v>46</v>
+      <c r="A47">
+        <v>582</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -995,8 +991,8 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
-        <v>47</v>
+      <c r="A48">
+        <v>583</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -1006,8 +1002,8 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
-        <v>48</v>
+      <c r="A49">
+        <v>587</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -1017,8 +1013,8 @@
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
-        <v>49</v>
+      <c r="A50">
+        <v>589</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -1028,8 +1024,8 @@
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
-        <v>50</v>
+      <c r="A51">
+        <v>591</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -1039,8 +1035,8 @@
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="1">
-        <v>51</v>
+      <c r="A52">
+        <v>594</v>
       </c>
       <c r="B52">
         <v>1</v>
@@ -1050,8 +1046,8 @@
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
-        <v>52</v>
+      <c r="A53">
+        <v>595</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -1061,8 +1057,8 @@
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
-        <v>53</v>
+      <c r="A54">
+        <v>596</v>
       </c>
       <c r="B54">
         <v>1</v>
@@ -1072,8 +1068,8 @@
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
-        <v>54</v>
+      <c r="A55">
+        <v>597</v>
       </c>
       <c r="B55">
         <v>1</v>
@@ -1083,96 +1079,96 @@
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
-        <v>55</v>
+      <c r="A56">
+        <v>501</v>
       </c>
       <c r="B56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
-        <v>56</v>
+      <c r="A57">
+        <v>502</v>
       </c>
       <c r="B57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
-        <v>57</v>
+      <c r="A58">
+        <v>503</v>
       </c>
       <c r="B58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="1">
-        <v>58</v>
+      <c r="A59">
+        <v>504</v>
       </c>
       <c r="B59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="1">
-        <v>59</v>
+      <c r="A60">
+        <v>505</v>
       </c>
       <c r="B60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="1">
-        <v>60</v>
+      <c r="A61">
+        <v>506</v>
       </c>
       <c r="B61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="1">
-        <v>61</v>
+      <c r="A62">
+        <v>507</v>
       </c>
       <c r="B62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="1">
-        <v>62</v>
+      <c r="A63">
+        <v>508</v>
       </c>
       <c r="B63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C63">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="1">
-        <v>63</v>
+      <c r="A64">
+        <v>509</v>
       </c>
       <c r="B64">
         <v>0</v>
@@ -1182,30 +1178,30 @@
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="1">
-        <v>64</v>
+      <c r="A65">
+        <v>514</v>
       </c>
       <c r="B65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C65">
         <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="1">
-        <v>65</v>
+      <c r="A66">
+        <v>515</v>
       </c>
       <c r="B66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C66">
         <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="1">
-        <v>66</v>
+      <c r="A67">
+        <v>519</v>
       </c>
       <c r="B67">
         <v>0</v>
@@ -1215,8 +1211,8 @@
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="1">
-        <v>67</v>
+      <c r="A68">
+        <v>520</v>
       </c>
       <c r="B68">
         <v>0</v>
@@ -1226,8 +1222,8 @@
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="1">
-        <v>68</v>
+      <c r="A69">
+        <v>521</v>
       </c>
       <c r="B69">
         <v>0</v>
@@ -1237,8 +1233,8 @@
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="1">
-        <v>69</v>
+      <c r="A70">
+        <v>522</v>
       </c>
       <c r="B70">
         <v>0</v>
@@ -1248,107 +1244,107 @@
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="1">
-        <v>70</v>
+      <c r="A71">
+        <v>523</v>
       </c>
       <c r="B71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C71">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="1">
-        <v>71</v>
+      <c r="A72">
+        <v>524</v>
       </c>
       <c r="B72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C72">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
-        <v>72</v>
+      <c r="A73">
+        <v>525</v>
       </c>
       <c r="B73">
         <v>1</v>
       </c>
       <c r="C73">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
-        <v>73</v>
+      <c r="A74">
+        <v>526</v>
       </c>
       <c r="B74">
         <v>1</v>
       </c>
       <c r="C74">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="1">
-        <v>74</v>
+      <c r="A75">
+        <v>527</v>
       </c>
       <c r="B75">
         <v>1</v>
       </c>
       <c r="C75">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="1">
-        <v>75</v>
+      <c r="A76">
+        <v>528</v>
       </c>
       <c r="B76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C76">
         <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="1">
-        <v>76</v>
+      <c r="A77">
+        <v>529</v>
       </c>
       <c r="B77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C77">
         <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="1">
-        <v>77</v>
+      <c r="A78">
+        <v>530</v>
       </c>
       <c r="B78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C78">
         <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="1">
-        <v>78</v>
+      <c r="A79">
+        <v>540</v>
       </c>
       <c r="B79">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C79">
         <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="1">
-        <v>79</v>
+      <c r="A80">
+        <v>563</v>
       </c>
       <c r="B80">
         <v>0</v>
@@ -1358,52 +1354,52 @@
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="1">
-        <v>80</v>
+      <c r="A81">
+        <v>564</v>
       </c>
       <c r="B81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="1">
-        <v>81</v>
+      <c r="A82">
+        <v>565</v>
       </c>
       <c r="B82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C82">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="1">
-        <v>82</v>
+      <c r="A83">
+        <v>566</v>
       </c>
       <c r="B83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C83">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="1">
-        <v>83</v>
+      <c r="A84">
+        <v>567</v>
       </c>
       <c r="B84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C84">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="1">
-        <v>84</v>
+      <c r="A85">
+        <v>568</v>
       </c>
       <c r="B85">
         <v>0</v>
@@ -1413,8 +1409,8 @@
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="1">
-        <v>85</v>
+      <c r="A86">
+        <v>569</v>
       </c>
       <c r="B86">
         <v>0</v>
@@ -1424,8 +1420,8 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="1">
-        <v>86</v>
+      <c r="A87">
+        <v>575</v>
       </c>
       <c r="B87">
         <v>0</v>
@@ -1435,41 +1431,41 @@
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="1">
-        <v>87</v>
+      <c r="A88">
+        <v>576</v>
       </c>
       <c r="B88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C88">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="1">
-        <v>88</v>
+      <c r="A89">
+        <v>577</v>
       </c>
       <c r="B89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C89">
         <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="1">
-        <v>89</v>
+      <c r="A90">
+        <v>578</v>
       </c>
       <c r="B90">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C90">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="1">
-        <v>90</v>
+      <c r="A91">
+        <v>579</v>
       </c>
       <c r="B91">
         <v>0</v>
@@ -1479,19 +1475,19 @@
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="1">
-        <v>91</v>
+      <c r="A92">
+        <v>584</v>
       </c>
       <c r="B92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C92">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="1">
-        <v>92</v>
+      <c r="A93">
+        <v>585</v>
       </c>
       <c r="B93">
         <v>0</v>
@@ -1501,8 +1497,8 @@
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="1">
-        <v>93</v>
+      <c r="A94">
+        <v>586</v>
       </c>
       <c r="B94">
         <v>0</v>
@@ -1512,52 +1508,52 @@
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="1">
-        <v>94</v>
+      <c r="A95">
+        <v>588</v>
       </c>
       <c r="B95">
         <v>1</v>
       </c>
       <c r="C95">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="1">
-        <v>95</v>
+      <c r="A96">
+        <v>590</v>
       </c>
       <c r="B96">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C96">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="1">
-        <v>96</v>
+      <c r="A97">
+        <v>592</v>
       </c>
       <c r="B97">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C97">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="1">
-        <v>97</v>
+      <c r="A98">
+        <v>593</v>
       </c>
       <c r="B98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C98">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="1">
-        <v>98</v>
+      <c r="A99">
+        <v>598</v>
       </c>
       <c r="B99">
         <v>0</v>
@@ -1567,8 +1563,8 @@
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="1">
-        <v>99</v>
+      <c r="A100">
+        <v>599</v>
       </c>
       <c r="B100">
         <v>0</v>
@@ -1578,8 +1574,8 @@
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="1">
-        <v>100</v>
+      <c r="A101">
+        <v>600</v>
       </c>
       <c r="B101">
         <v>0</v>
@@ -1589,8 +1585,8 @@
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="1">
-        <v>101</v>
+      <c r="A102">
+        <v>601</v>
       </c>
       <c r="B102">
         <v>0</v>
@@ -1600,8 +1596,8 @@
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="1">
-        <v>102</v>
+      <c r="A103">
+        <v>602</v>
       </c>
       <c r="B103">
         <v>0</v>
@@ -1611,8 +1607,8 @@
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="1">
-        <v>103</v>
+      <c r="A104">
+        <v>603</v>
       </c>
       <c r="B104">
         <v>0</v>
@@ -1622,8 +1618,8 @@
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="1">
-        <v>104</v>
+      <c r="A105">
+        <v>604</v>
       </c>
       <c r="B105">
         <v>0</v>
@@ -1633,8 +1629,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C105">
-    <sortCondition ref="A1:A105"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C106">
+    <sortCondition ref="C1:C106"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1645,7 +1641,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1655,7 +1651,7 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1700,7 +1696,7 @@
   <dimension ref="A1:B58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1714,456 +1710,456 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>14</v>
+      <c r="A2">
+        <v>514</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>15</v>
+      <c r="A3">
+        <v>515</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>25</v>
+      <c r="A4">
+        <v>525</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>26</v>
+      <c r="A5">
+        <v>526</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>27</v>
+      <c r="A6">
+        <v>527</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>28</v>
+      <c r="A7">
+        <v>528</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>29</v>
+      <c r="A8">
+        <v>529</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>30</v>
+      <c r="A9">
+        <v>530</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>31</v>
+      <c r="A10">
+        <v>531</v>
       </c>
       <c r="B10">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>32</v>
+      <c r="A11">
+        <v>532</v>
       </c>
       <c r="B11">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>33</v>
+      <c r="A12">
+        <v>533</v>
       </c>
       <c r="B12">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>34</v>
+      <c r="A13">
+        <v>534</v>
       </c>
       <c r="B13">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>35</v>
+      <c r="A14">
+        <v>535</v>
       </c>
       <c r="B14">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>36</v>
+      <c r="A15">
+        <v>536</v>
       </c>
       <c r="B15">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>37</v>
+      <c r="A16">
+        <v>537</v>
       </c>
       <c r="B16">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>38</v>
+      <c r="A17">
+        <v>538</v>
       </c>
       <c r="B17">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>39</v>
+      <c r="A18">
+        <v>539</v>
       </c>
       <c r="B18">
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>40</v>
+      <c r="A19">
+        <v>540</v>
       </c>
       <c r="B19">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>41</v>
+      <c r="A20">
+        <v>541</v>
       </c>
       <c r="B20">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>42</v>
+      <c r="A21">
+        <v>542</v>
       </c>
       <c r="B21">
         <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>43</v>
+      <c r="A22">
+        <v>543</v>
       </c>
       <c r="B22">
         <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>44</v>
+      <c r="A23">
+        <v>544</v>
       </c>
       <c r="B23">
         <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>45</v>
+      <c r="A24">
+        <v>545</v>
       </c>
       <c r="B24">
         <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>46</v>
+      <c r="A25">
+        <v>546</v>
       </c>
       <c r="B25">
         <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>47</v>
+      <c r="A26">
+        <v>547</v>
       </c>
       <c r="B26">
         <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>48</v>
+      <c r="A27">
+        <v>548</v>
       </c>
       <c r="B27">
         <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>49</v>
+      <c r="A28">
+        <v>549</v>
       </c>
       <c r="B28">
         <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>50</v>
+      <c r="A29">
+        <v>550</v>
       </c>
       <c r="B29">
         <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>51</v>
+      <c r="A30">
+        <v>551</v>
       </c>
       <c r="B30">
         <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>52</v>
+      <c r="A31">
+        <v>552</v>
       </c>
       <c r="B31">
         <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>53</v>
+      <c r="A32">
+        <v>553</v>
       </c>
       <c r="B32">
         <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>54</v>
+      <c r="A33">
+        <v>554</v>
       </c>
       <c r="B33">
         <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>55</v>
+      <c r="A34">
+        <v>555</v>
       </c>
       <c r="B34">
         <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>56</v>
+      <c r="A35">
+        <v>556</v>
       </c>
       <c r="B35">
         <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>57</v>
+      <c r="A36">
+        <v>557</v>
       </c>
       <c r="B36">
         <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <v>58</v>
+      <c r="A37">
+        <v>558</v>
       </c>
       <c r="B37">
         <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
-        <v>59</v>
+      <c r="A38">
+        <v>559</v>
       </c>
       <c r="B38">
         <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <v>60</v>
+      <c r="A39">
+        <v>560</v>
       </c>
       <c r="B39">
         <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
-        <v>61</v>
+      <c r="A40">
+        <v>561</v>
       </c>
       <c r="B40">
         <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <v>62</v>
+      <c r="A41">
+        <v>562</v>
       </c>
       <c r="B41">
         <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
-        <v>70</v>
+      <c r="A42">
+        <v>570</v>
       </c>
       <c r="B42">
         <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
-        <v>71</v>
+      <c r="A43">
+        <v>571</v>
       </c>
       <c r="B43">
         <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
-        <v>72</v>
+      <c r="A44">
+        <v>572</v>
       </c>
       <c r="B44">
         <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
-        <v>73</v>
+      <c r="A45">
+        <v>573</v>
       </c>
       <c r="B45">
         <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
-        <v>74</v>
+      <c r="A46">
+        <v>574</v>
       </c>
       <c r="B46">
         <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
-        <v>80</v>
+      <c r="A47">
+        <v>580</v>
       </c>
       <c r="B47">
         <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
-        <v>81</v>
+      <c r="A48">
+        <v>581</v>
       </c>
       <c r="B48">
         <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
-        <v>82</v>
+      <c r="A49">
+        <v>582</v>
       </c>
       <c r="B49">
         <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
-        <v>83</v>
+      <c r="A50">
+        <v>583</v>
       </c>
       <c r="B50">
         <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
-        <v>87</v>
+      <c r="A51">
+        <v>587</v>
       </c>
       <c r="B51">
         <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="1">
-        <v>88</v>
+      <c r="A52">
+        <v>588</v>
       </c>
       <c r="B52">
         <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
-        <v>89</v>
+      <c r="A53">
+        <v>589</v>
       </c>
       <c r="B53">
         <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
-        <v>91</v>
+      <c r="A54">
+        <v>591</v>
       </c>
       <c r="B54">
         <v>4</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
-        <v>94</v>
+      <c r="A55">
+        <v>594</v>
       </c>
       <c r="B55">
         <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
-        <v>95</v>
+      <c r="A56">
+        <v>595</v>
       </c>
       <c r="B56">
         <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
-        <v>96</v>
+      <c r="A57">
+        <v>596</v>
       </c>
       <c r="B57">
         <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
-        <v>97</v>
+      <c r="A58">
+        <v>597</v>
       </c>
       <c r="B58">
         <v>4</v>
@@ -2178,7 +2174,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A0B0A54-EBD8-4483-8003-BDECA55AA08A}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -2187,7 +2185,7 @@
         <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2195,7 +2193,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2203,7 +2201,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2211,7 +2209,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2219,7 +2217,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2227,7 +2225,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2235,7 +2233,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2243,7 +2241,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -2255,8 +2253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{550B3CE6-B11A-4F82-9FAE-C2294524CC09}">
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2270,400 +2268,400 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
+      <c r="A2">
+        <v>501</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
+      <c r="A3">
+        <v>502</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
+      <c r="A4">
+        <v>503</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
+      <c r="A5">
+        <v>504</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
+      <c r="A6">
+        <v>505</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
+      <c r="A7">
+        <v>506</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7</v>
+      <c r="A8">
+        <v>507</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>8</v>
+      <c r="A9">
+        <v>508</v>
       </c>
       <c r="B9">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>9</v>
+      <c r="A10">
+        <v>509</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>14</v>
+      <c r="A11">
+        <v>514</v>
       </c>
       <c r="B11">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>15</v>
+      <c r="A12">
+        <v>515</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>19</v>
+      <c r="A13">
+        <v>519</v>
       </c>
       <c r="B13">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>20</v>
+      <c r="A14">
+        <v>520</v>
       </c>
       <c r="B14">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>21</v>
+      <c r="A15">
+        <v>521</v>
       </c>
       <c r="B15">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>22</v>
+      <c r="A16">
+        <v>522</v>
       </c>
       <c r="B16">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>23</v>
+      <c r="A17">
+        <v>523</v>
       </c>
       <c r="B17">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>24</v>
+      <c r="A18">
+        <v>524</v>
       </c>
       <c r="B18">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>25</v>
+      <c r="A19">
+        <v>525</v>
       </c>
       <c r="B19">
         <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>26</v>
+      <c r="A20">
+        <v>526</v>
       </c>
       <c r="B20">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>27</v>
+      <c r="A21">
+        <v>527</v>
       </c>
       <c r="B21">
         <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>28</v>
+      <c r="A22">
+        <v>528</v>
       </c>
       <c r="B22">
         <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>29</v>
+      <c r="A23">
+        <v>529</v>
       </c>
       <c r="B23">
         <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>30</v>
+      <c r="A24">
+        <v>530</v>
       </c>
       <c r="B24">
         <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>40</v>
+      <c r="A25">
+        <v>540</v>
       </c>
       <c r="B25">
         <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>63</v>
+      <c r="A26">
+        <v>563</v>
       </c>
       <c r="B26">
         <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>64</v>
+      <c r="A27">
+        <v>564</v>
       </c>
       <c r="B27">
         <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>65</v>
+      <c r="A28">
+        <v>565</v>
       </c>
       <c r="B28">
         <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>66</v>
+      <c r="A29">
+        <v>566</v>
       </c>
       <c r="B29">
         <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>67</v>
+      <c r="A30">
+        <v>567</v>
       </c>
       <c r="B30">
         <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>68</v>
+      <c r="A31">
+        <v>568</v>
       </c>
       <c r="B31">
         <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>69</v>
+      <c r="A32">
+        <v>569</v>
       </c>
       <c r="B32">
         <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>75</v>
+      <c r="A33">
+        <v>575</v>
       </c>
       <c r="B33">
         <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>76</v>
+      <c r="A34">
+        <v>576</v>
       </c>
       <c r="B34">
         <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>77</v>
+      <c r="A35">
+        <v>577</v>
       </c>
       <c r="B35">
         <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>78</v>
+      <c r="A36">
+        <v>578</v>
       </c>
       <c r="B36">
         <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <v>79</v>
+      <c r="A37">
+        <v>579</v>
       </c>
       <c r="B37">
         <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
-        <v>84</v>
+      <c r="A38">
+        <v>584</v>
       </c>
       <c r="B38">
         <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <v>85</v>
+      <c r="A39">
+        <v>585</v>
       </c>
       <c r="B39">
         <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
-        <v>86</v>
+      <c r="A40">
+        <v>586</v>
       </c>
       <c r="B40">
         <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <v>88</v>
+      <c r="A41">
+        <v>588</v>
       </c>
       <c r="B41">
         <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
-        <v>90</v>
+      <c r="A42">
+        <v>590</v>
       </c>
       <c r="B42">
         <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
-        <v>92</v>
+      <c r="A43">
+        <v>592</v>
       </c>
       <c r="B43">
         <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
-        <v>93</v>
+      <c r="A44">
+        <v>593</v>
       </c>
       <c r="B44">
         <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
-        <v>98</v>
+      <c r="A45">
+        <v>598</v>
       </c>
       <c r="B45">
         <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
-        <v>99</v>
+      <c r="A46">
+        <v>599</v>
       </c>
       <c r="B46">
         <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
-        <v>100</v>
+      <c r="A47">
+        <v>600</v>
       </c>
       <c r="B47">
         <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
-        <v>101</v>
+      <c r="A48">
+        <v>601</v>
       </c>
       <c r="B48">
         <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
-        <v>102</v>
+      <c r="A49">
+        <v>602</v>
       </c>
       <c r="B49">
         <v>5</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
-        <v>103</v>
+      <c r="A50">
+        <v>603</v>
       </c>
       <c r="B50">
         <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
-        <v>104</v>
+      <c r="A51">
+        <v>604</v>
       </c>
       <c r="B51">
         <v>5</v>

</xml_diff>